<commit_message>
Included Special Pins Of TM4C123Gh6PM in the sheet
</commit_message>
<xml_diff>
--- a/FireBird Board Pin Out.xlsx
+++ b/FireBird Board Pin Out.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="188">
   <si>
     <t>Pin Out</t>
   </si>
@@ -391,6 +391,195 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>PIN No</t>
+  </si>
+  <si>
+    <t>Special Comments</t>
+  </si>
+  <si>
+    <t>PE 0</t>
+  </si>
+  <si>
+    <t>PE1</t>
+  </si>
+  <si>
+    <t>PE2</t>
+  </si>
+  <si>
+    <t>PE3</t>
+  </si>
+  <si>
+    <t>PD0</t>
+  </si>
+  <si>
+    <t>PD1</t>
+  </si>
+  <si>
+    <t>PD2</t>
+  </si>
+  <si>
+    <t>PD3</t>
+  </si>
+  <si>
+    <t>PE4</t>
+  </si>
+  <si>
+    <t>PE5</t>
+  </si>
+  <si>
+    <t>PB4</t>
+  </si>
+  <si>
+    <t>PB5</t>
+  </si>
+  <si>
+    <t>UART</t>
+  </si>
+  <si>
+    <t>PROGRAMMER UART</t>
+  </si>
+  <si>
+    <t>PA0 RX0</t>
+  </si>
+  <si>
+    <t>PA1 TX0</t>
+  </si>
+  <si>
+    <t>PC4,PB0 RX1</t>
+  </si>
+  <si>
+    <t>PC5,PB1 TX1</t>
+  </si>
+  <si>
+    <t>PD6 RX2</t>
+  </si>
+  <si>
+    <t>PD7 TX2</t>
+  </si>
+  <si>
+    <t>PC6 RX3</t>
+  </si>
+  <si>
+    <t>PC7 RX3</t>
+  </si>
+  <si>
+    <t>PC4 RX</t>
+  </si>
+  <si>
+    <t>PC5 TX4</t>
+  </si>
+  <si>
+    <t>PE4 RX5</t>
+  </si>
+  <si>
+    <t>PE5 TX5</t>
+  </si>
+  <si>
+    <t>PD4 RX6</t>
+  </si>
+  <si>
+    <t>PD5 TX6</t>
+  </si>
+  <si>
+    <t>PE0 RX7</t>
+  </si>
+  <si>
+    <t>PE1 RX7</t>
+  </si>
+  <si>
+    <t>TM4C123gh6PM Special Pins.</t>
+  </si>
+  <si>
+    <t>PWM</t>
+  </si>
+  <si>
+    <t>PIN Name</t>
+  </si>
+  <si>
+    <t>Pin</t>
+  </si>
+  <si>
+    <t>Generator</t>
+  </si>
+  <si>
+    <t>M0PWM0</t>
+  </si>
+  <si>
+    <t>M0PWM1</t>
+  </si>
+  <si>
+    <t>M0PWM2</t>
+  </si>
+  <si>
+    <t>M0PWM3</t>
+  </si>
+  <si>
+    <t>M0PWM4</t>
+  </si>
+  <si>
+    <t>MOPWM5</t>
+  </si>
+  <si>
+    <t>M0PWM6</t>
+  </si>
+  <si>
+    <t>M0PWM7</t>
+  </si>
+  <si>
+    <t>M1PWM0</t>
+  </si>
+  <si>
+    <t>M1PWM1</t>
+  </si>
+  <si>
+    <t>M1PWM2</t>
+  </si>
+  <si>
+    <t>M1PWM3</t>
+  </si>
+  <si>
+    <t>M1PWM4</t>
+  </si>
+  <si>
+    <t>M1PWM5</t>
+  </si>
+  <si>
+    <t>M1PWM6</t>
+  </si>
+  <si>
+    <t>M1PWM7</t>
+  </si>
+  <si>
+    <t>PB6</t>
+  </si>
+  <si>
+    <t>PB7</t>
+  </si>
+  <si>
+    <t>PC4,PD0</t>
+  </si>
+  <si>
+    <t>PC5,PD1</t>
+  </si>
+  <si>
+    <t>PA6 PE4</t>
+  </si>
+  <si>
+    <t>PA7 PE5</t>
+  </si>
+  <si>
+    <t>PF0</t>
+  </si>
+  <si>
+    <t>PF1</t>
+  </si>
+  <si>
+    <t>PF2</t>
+  </si>
+  <si>
+    <t>PF3</t>
   </si>
 </sst>
 </file>
@@ -735,10 +924,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F75"/>
+  <dimension ref="A1:F124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1609,6 +1798,361 @@
       </c>
       <c r="D75" t="s">
         <v>93</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>125</v>
+      </c>
+      <c r="C78" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>46</v>
+      </c>
+      <c r="B79" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>139</v>
+      </c>
+      <c r="B91" t="s">
+        <v>141</v>
+      </c>
+      <c r="C91" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
+        <v>142</v>
+      </c>
+      <c r="C92" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B94" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B95" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B97" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B98" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B99" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B100" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B101" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B102" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B103" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B104" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B105" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B106" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>158</v>
+      </c>
+      <c r="B107" t="s">
+        <v>159</v>
+      </c>
+      <c r="C107" t="s">
+        <v>160</v>
+      </c>
+      <c r="D107" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B108" t="s">
+        <v>162</v>
+      </c>
+      <c r="C108" t="s">
+        <v>178</v>
+      </c>
+      <c r="D108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B109" t="s">
+        <v>163</v>
+      </c>
+      <c r="C109" t="s">
+        <v>179</v>
+      </c>
+      <c r="D109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B110" t="s">
+        <v>164</v>
+      </c>
+      <c r="C110" t="s">
+        <v>137</v>
+      </c>
+      <c r="D110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B112" t="s">
+        <v>165</v>
+      </c>
+      <c r="C112" t="s">
+        <v>138</v>
+      </c>
+      <c r="D112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B113" t="s">
+        <v>166</v>
+      </c>
+      <c r="C113" t="s">
+        <v>135</v>
+      </c>
+      <c r="D113">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B114" t="s">
+        <v>167</v>
+      </c>
+      <c r="C114" t="s">
+        <v>136</v>
+      </c>
+      <c r="D114">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="115" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B115" t="s">
+        <v>168</v>
+      </c>
+      <c r="C115" t="s">
+        <v>180</v>
+      </c>
+      <c r="D115">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="116" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B116" t="s">
+        <v>169</v>
+      </c>
+      <c r="C116" t="s">
+        <v>181</v>
+      </c>
+      <c r="D116">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="117" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B117" t="s">
+        <v>170</v>
+      </c>
+      <c r="C117" t="s">
+        <v>131</v>
+      </c>
+      <c r="D117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B118" t="s">
+        <v>171</v>
+      </c>
+      <c r="C118" t="s">
+        <v>132</v>
+      </c>
+      <c r="D118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B119" t="s">
+        <v>172</v>
+      </c>
+      <c r="C119" t="s">
+        <v>182</v>
+      </c>
+      <c r="D119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B120" t="s">
+        <v>173</v>
+      </c>
+      <c r="C120" t="s">
+        <v>183</v>
+      </c>
+      <c r="D120">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B121" t="s">
+        <v>174</v>
+      </c>
+      <c r="C121" t="s">
+        <v>184</v>
+      </c>
+      <c r="D121">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="122" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B122" t="s">
+        <v>175</v>
+      </c>
+      <c r="C122" t="s">
+        <v>185</v>
+      </c>
+      <c r="D122">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="123" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B123" t="s">
+        <v>176</v>
+      </c>
+      <c r="C123" t="s">
+        <v>186</v>
+      </c>
+      <c r="D123">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="124" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B124" t="s">
+        <v>177</v>
+      </c>
+      <c r="C124" t="s">
+        <v>187</v>
+      </c>
+      <c r="D124">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Codes for velocity control
</commit_message>
<xml_diff>
--- a/FireBird Board Pin Out.xlsx
+++ b/FireBird Board Pin Out.xlsx
@@ -1241,8 +1241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A134" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C155" sqref="C155"/>
+    <sheetView tabSelected="1" topLeftCell="D33" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>